<commit_message>
Updating do files and support files
Updating do files and support files
</commit_message>
<xml_diff>
--- a/documentation/SSGD v2.0 codebook.xlsx
+++ b/documentation/SSGD v2.0 codebook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Omar\World Bank\SSG database\paper\figures_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E367F9D-17B7-428C-AA04-E6F45ABD4AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B034F253-4ED6-4CC9-8DC7-A6CD352235B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{39A305B4-F82F-4338-8C8F-A8E3E187CC91}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{39A305B4-F82F-4338-8C8F-A8E3E187CC91}"/>
   </bookViews>
   <sheets>
     <sheet name="Social Inclusion" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="521">
   <si>
     <t>Dimension</t>
   </si>
@@ -300,9 +300,6 @@
     <t>GMD: Uses the harmonised variable "socialsec" (social security status) which has 2 values
 0 = No
 1 = Yes</t>
-  </si>
-  <si>
-    <t>Women, Business and the Law (WBL) score</t>
   </si>
   <si>
     <t>wbl_index</t>
@@ -1277,12 +1274,6 @@
     <t>rullaw</t>
   </si>
   <si>
-    <t>Rule of Law index</t>
-  </si>
-  <si>
-    <t>WGI: Rule of law index</t>
-  </si>
-  <si>
     <t>WGI</t>
   </si>
   <si>
@@ -1304,12 +1295,6 @@
     <t>goveff</t>
   </si>
   <si>
-    <t>Government effectiveness index</t>
-  </si>
-  <si>
-    <t>WGI: Government effectiveness index</t>
-  </si>
-  <si>
     <r>
       <t>Control of corruption</t>
     </r>
@@ -1328,12 +1313,6 @@
     <t>concor</t>
   </si>
   <si>
-    <t>Control of corruption index</t>
-  </si>
-  <si>
-    <t>WGI: Control of corruption index</t>
-  </si>
-  <si>
     <r>
       <t>Voice and accountability</t>
     </r>
@@ -1352,12 +1331,6 @@
     <t>voiceest</t>
   </si>
   <si>
-    <t>Voice and accountability index</t>
-  </si>
-  <si>
-    <t>Economic and social rights performance score</t>
-  </si>
-  <si>
     <t>econsocrights</t>
   </si>
   <si>
@@ -1379,12 +1352,6 @@
     <t>riggua</t>
   </si>
   <si>
-    <t>Life and security are effectively guaranteed score</t>
-  </si>
-  <si>
-    <t>WJP: Fundamental Rights - The right to life and security of the person is effectively guaranteed score</t>
-  </si>
-  <si>
     <t>WJP</t>
   </si>
   <si>
@@ -1406,12 +1373,6 @@
     <t>powlim</t>
   </si>
   <si>
-    <t>Government power are limited by the judiciary score</t>
-  </si>
-  <si>
-    <t>WJP: Constraints on Government Powers - Government powers are effectively limited by the judiciary</t>
-  </si>
-  <si>
     <r>
       <t>Equal treatment and absence of discrimination</t>
     </r>
@@ -1430,12 +1391,6 @@
     <t>nodis</t>
   </si>
   <si>
-    <t>Equal treatment and absence of discrimination score</t>
-  </si>
-  <si>
-    <t>WJP: Fundamental Rights - Equal treatment and absence of discrimination</t>
-  </si>
-  <si>
     <r>
       <t>Government regulations are applied and enforced without improper influence</t>
     </r>
@@ -1454,12 +1409,6 @@
     <t>govreg</t>
   </si>
   <si>
-    <t>Government regulations are applied and enforced without improper influence score</t>
-  </si>
-  <si>
-    <t>WJP: Regulatory Enforcement - Government regulations are applied and enforced without improper influence</t>
-  </si>
-  <si>
     <r>
       <t>People can access and afford civil justice</t>
     </r>
@@ -1478,12 +1427,6 @@
     <t>accjus</t>
   </si>
   <si>
-    <t>People can access and afford civil justice</t>
-  </si>
-  <si>
-    <t>WJP: Civil Justice - People can access and afford civil justice</t>
-  </si>
-  <si>
     <r>
       <t>Civic space score</t>
     </r>
@@ -1502,12 +1445,6 @@
     <t>civspa</t>
   </si>
   <si>
-    <t>Civic space score</t>
-  </si>
-  <si>
-    <t>CIVICUS: Civic space score</t>
-  </si>
-  <si>
     <t>CIVICUS</t>
   </si>
   <si>
@@ -1518,9 +1455,6 @@
   </si>
   <si>
     <t>The Democracy Index is an index measuring the quality of democracy across the world. Is centrally concerned with democratic rights and democratic institutions.</t>
-  </si>
-  <si>
-    <t>EIU: The Democracy Index is an index measuring the quality of democracy across the world. Is centrally concerned with democratic rights and democratic institutions.</t>
   </si>
   <si>
     <t>EIU</t>
@@ -1666,12 +1600,6 @@
     <t>Fatalities due to violence</t>
   </si>
   <si>
-    <t>WGI: Voice and accountability index</t>
-  </si>
-  <si>
-    <t>WGI: Economic and social rights performance score</t>
-  </si>
-  <si>
     <r>
       <t>Women, Business and the Law (WBL) score</t>
     </r>
@@ -1837,39 +1765,24 @@
     <t>ex_ageg1</t>
   </si>
   <si>
-    <t>% aged 15-29</t>
-  </si>
-  <si>
     <t>Share of population aged 15 to 29 years old</t>
   </si>
   <si>
     <t>ex_ageg2</t>
   </si>
   <si>
-    <t>% aged 30-59</t>
-  </si>
-  <si>
     <t>Share of population aged 30 to 59 years old</t>
   </si>
   <si>
     <t>ex_ageg3</t>
   </si>
   <si>
-    <t>% aged 60+</t>
-  </si>
-  <si>
     <t>Share of population aged 60+ years old</t>
   </si>
   <si>
     <t>ex_avega2</t>
   </si>
   <si>
-    <t>Inequality of opportunities</t>
-  </si>
-  <si>
-    <t>Average value of the following rates: i) Birth registration, ii) Enrollment in preschool, iii) Survival at age 5, and iv) Equal remuneration for females doing equal work than males</t>
-  </si>
-  <si>
     <t>ex_co2emissions</t>
   </si>
   <si>
@@ -1891,18 +1804,12 @@
     <t>ex_disability1</t>
   </si>
   <si>
-    <t>% who experienced discrimination based on disability</t>
-  </si>
-  <si>
     <t>Percentage of people who experienced discrimination based on disability</t>
   </si>
   <si>
     <t>ex_disability2</t>
   </si>
   <si>
-    <t>% who have at least one household member living with disabilities</t>
-  </si>
-  <si>
     <t>Percentage of people who have at least one household member living with disabilities</t>
   </si>
   <si>
@@ -1966,9 +1873,6 @@
     <t>Inequality of opportunities, using HCI</t>
   </si>
   <si>
-    <t>Gap between human capital index male and female</t>
-  </si>
-  <si>
     <t>ex_gdpppc</t>
   </si>
   <si>
@@ -2020,9 +1924,6 @@
     <t>ex_sex</t>
   </si>
   <si>
-    <t>% of male pop</t>
-  </si>
-  <si>
     <t>Share of male population</t>
   </si>
   <si>
@@ -2050,15 +1951,9 @@
     <t>Tree cover loss</t>
   </si>
   <si>
-    <t>Tree Cover Loss</t>
-  </si>
-  <si>
     <t>ex_urbpop</t>
   </si>
   <si>
-    <t>% of urban pop</t>
-  </si>
-  <si>
     <t>Share of population living in urban areas</t>
   </si>
   <si>
@@ -2074,9 +1969,6 @@
     <t>ex_youth</t>
   </si>
   <si>
-    <t>% aged 15-24 (w.r.t 15+ pop)</t>
-  </si>
-  <si>
     <t>Share of population aged 15 to 24 years old (w.r.t. 15+ years old population)</t>
   </si>
   <si>
@@ -2113,9 +2005,6 @@
     <t>ex_polstab</t>
   </si>
   <si>
-    <t xml:space="preserve">	Political Stability and Absence of Violence/Terrorism: Estimate</t>
-  </si>
-  <si>
     <t xml:space="preserve">	Political Stability and Absence of Violence/Terrorism measures perceptions of the likelihood of political instability and/or politically-motivated violence, including terrorism.</t>
   </si>
   <si>
@@ -2129,9 +2018,6 @@
   </si>
   <si>
     <t>ex_regulqua</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	Regulatory Quality: Estimate</t>
   </si>
   <si>
     <t>ex_researchexp</t>
@@ -2193,22 +2079,7 @@
 Numeric [0-10]</t>
   </si>
   <si>
-    <t>WDI: Gap between human capital index male and female</t>
-  </si>
-  <si>
-    <t>WDI: The shared prosperity premium is defined as the difference between the annualized growth in the average consumption or income per capita of the poorest 40 percent and the entire population</t>
-  </si>
-  <si>
-    <t>WDI: Shared prosperity is defined as the annualized growth rate in the average consumption or income per capita of the poorest 40 percent (the bottom 40) of the population in a country. It measures the extent to which economic growth is inclusive by focusing on household consumption or income growth among the poorest population rather than on growth in the average.</t>
-  </si>
-  <si>
     <t>GMD: Age of respondent</t>
-  </si>
-  <si>
-    <t>ESG: CO2 emissions in metric tons per capita</t>
-  </si>
-  <si>
-    <t>ESG: Number of degrees that a day's average temperature is above 18.3°C</t>
   </si>
   <si>
     <t>Energy intensity level of primary energy is the ratio between energy supply and gross domestic product measured at purchasing power parity. Energy intensity is an indication of how much energy is used to produce one unit of economic output. Lower ratio indicates that less energy is used to produce one unit of output.</t>
@@ -2293,16 +2164,145 @@
     <t>ESG: Unmet need for contraception (% of married women ages 15-49)</t>
   </si>
   <si>
-    <t>WGI: Political Stability and Absence of Violence/Terrorism: Estimate</t>
-  </si>
-  <si>
-    <t>WGI: Regulatory Quality: Estimate</t>
-  </si>
-  <si>
     <t>WDI: GDP growth (annual %)</t>
   </si>
   <si>
     <t>ESG: Level of water stress</t>
+  </si>
+  <si>
+    <t>% of pop aged 15-29</t>
+  </si>
+  <si>
+    <t>% of pop aged 30-59</t>
+  </si>
+  <si>
+    <t>% of pop aged 60+</t>
+  </si>
+  <si>
+    <t>Inequality of opportunities index</t>
+  </si>
+  <si>
+    <t>% of pop who experienced discrimination based on disability</t>
+  </si>
+  <si>
+    <t>% of pop who have at least one household member living with disabilities</t>
+  </si>
+  <si>
+    <t>The Human Development Index (HDI) is a summary measure of average achievement in key dimensions of human development: a long and healthy life, being knowledgeable and having a decent standard of living. The HDI is the geometric mean of normalized indices for each of the three dimensions.</t>
+  </si>
+  <si>
+    <t>% of male population</t>
+  </si>
+  <si>
+    <t>The Economic and Social Rights Performance Score reflects how well countries are fulfilling their citizens' economic and social rights. This score evaluates performance based on the rights to food, education, health, housing, and work, taking into account a country’s income level to provide a fair comparison across different economic contexts.</t>
+  </si>
+  <si>
+    <t>The inequality of opportunities index is computed as the gap in the Human Capital Index between males and females.</t>
+  </si>
+  <si>
+    <t>The Tree Cover Loss indicator shows year-by-year tree cover loss, defined as stand level replacement of vegetation greater than 5 meters, within the selected area. The tree cover loss data set is a collaboration of the University of Maryland, Google, USGS, and NASA, and uses Landsat satellite images to map annual tree cover loss at a 30 × 30 meter resolution. Note that “tree cover loss” is not the same as “deforestation” – tree cover loss includes change in both natural and planted forest, and does not need to be human caused. The data from 2011 onward were produced with an updated methodology that may capture additional loss. Comparisons between the original 2001-2010 data and future years should be performed with caution.</t>
+  </si>
+  <si>
+    <t>% of urban population</t>
+  </si>
+  <si>
+    <t>% of pop aged 15-24 (w.r.t 15+ pop)</t>
+  </si>
+  <si>
+    <t>This indicator measures the accessibility and affordability of civil courts, including whether people are aware of available remedies; can access and afford legal advice and representation; and can access the court system without incurring unreasonable fees, encountering unreasonable procedural hurdles, or experiencing physical or linguistic barriers.</t>
+  </si>
+  <si>
+    <t>Control of corruption captures perceptions of the extent to which public power is exercised for private gain, including both petty and grand forms of corruption, as well as "capture" of the state by elites and private interests.</t>
+  </si>
+  <si>
+    <t>Government effectiveness captures perceptions of the quality of public services, the quality of the civil service and the degree of its independence from political pressures, the quality of policy formulation and implementation, and the credibility of the government's commitment to such policies.</t>
+  </si>
+  <si>
+    <t>This indicator measures whether individuals are free from discrimination—based on socio-economic status, gender, ethnicity, religion, national origin, sexual orientation, or gender identity—with respect to public services, employment, court proceedings, and the justice system.</t>
+  </si>
+  <si>
+    <t>This indicator measures whether the enforcement of regulations is subject to bribery or improper influence by private interests, and whether public services, such as the issuance of permits and licenses and the administration of public health services, are provided without bribery or other inducements.</t>
+  </si>
+  <si>
+    <t>This indicator measures whether the judiciary has the independence and the ability in practice to exercise effective checks on the government.</t>
+  </si>
+  <si>
+    <t>This indicator measures whether the police inflict physical harm upon criminal suspects during arrest and interrogation, and whether political dissidents or members of the media are subjected to unreasonable searches, arrest, detention, imprisonment, threats, abusive treatment, or violence.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rule of law captures perceptions of the extent to which agents have confidence in and abide by the rules of society, and in particular the quality of contract enforcement, property rights, the police, and the courts, as well as the likelihood of crime and violence. </t>
+  </si>
+  <si>
+    <t>Voice and accountability captures perceptions of the extent to which a country's citizens are able to participate in selecting their government, as well as freedom of expression, freedom of association, and a free media.</t>
+  </si>
+  <si>
+    <t>The Women, Business, and the Law score measures how laws and regulations affect women's economic opportunity in 190 economies. It assesses areas such as mobility, workplace rights, pay, marriage, parenthood, entrepreneurship, assets, and pension, providing a score that reflects the degree to which a nation's legal framework supports women's economic participation.</t>
+  </si>
+  <si>
+    <t>WBL: The Women, Business, and the Law score measures how laws and regulations affect women's economic opportunity in 190 economies. It assesses areas such as mobility, workplace rights, pay, marriage, parenthood, entrepreneurship, assets, and pension, providing a score that reflects the degree to which a nation's legal framework supports women's economic participation.</t>
+  </si>
+  <si>
+    <t>The Civic Space Score measures the state of civic freedoms in a country, specifically evaluating the conditions for civil society based on three fundamental dimensions: freedom of association, freedom of peaceful assembly, and freedom of expression. This score helps to assess whether citizens are able to engage and communicate without undue interference or repression by the state.</t>
+  </si>
+  <si>
+    <t>Regulatory Quality: Estimate</t>
+  </si>
+  <si>
+    <t>Political Stability and Absence of Violence/Terrorism: Estimate</t>
+  </si>
+  <si>
+    <t>WGI: Regulatory Quality estimate</t>
+  </si>
+  <si>
+    <t>WGI: Political Stability and Absence of Violence/Terrorism estimate</t>
+  </si>
+  <si>
+    <t>ESG: The Tree Cover Loss</t>
+  </si>
+  <si>
+    <t>ESG: CO2 emissions</t>
+  </si>
+  <si>
+    <t>ESG: Cooling degree days</t>
+  </si>
+  <si>
+    <t>EIU: Democracy Index</t>
+  </si>
+  <si>
+    <t>CIVICUS: Civic Space Score</t>
+  </si>
+  <si>
+    <t>WJP: People can access and afford civil justice</t>
+  </si>
+  <si>
+    <t>WJP: Government regulations are applied and enforced without improper influence</t>
+  </si>
+  <si>
+    <t>WJP: Equal treatment and absence of discrimination</t>
+  </si>
+  <si>
+    <t>WJP: Government powers are limited by the judiciary</t>
+  </si>
+  <si>
+    <t>WJP: Life and security are effectively guaranteed</t>
+  </si>
+  <si>
+    <t>Economic and Social Rights Performance Score</t>
+  </si>
+  <si>
+    <t>ESG: Economic and Social Rights Performance Score</t>
+  </si>
+  <si>
+    <t>WGI: Voice and accountability</t>
+  </si>
+  <si>
+    <t>WGI: Control of corruption</t>
+  </si>
+  <si>
+    <t>WGI: Government effectiveness</t>
+  </si>
+  <si>
+    <t>WGI: Rule of law</t>
   </si>
 </sst>
 </file>
@@ -2797,7 +2797,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6076DEB1-9DD4-4009-8CB4-9AD827C47535}">
   <dimension ref="B2:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2937,10 +2939,10 @@
         <v>27</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>351</v>
+        <v>329</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>365</v>
+        <v>341</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="60" x14ac:dyDescent="0.25">
@@ -3137,196 +3139,196 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="105" x14ac:dyDescent="0.25">
       <c r="B19" s="22"/>
       <c r="C19" s="22" t="s">
-        <v>350</v>
+        <v>328</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>355</v>
+        <v>331</v>
       </c>
       <c r="E19" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>498</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="H19" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
       <c r="D20" s="6" t="s">
-        <v>357</v>
+        <v>333</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B21" s="22"/>
       <c r="C21" s="22"/>
       <c r="D21" s="6" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B22" s="22"/>
       <c r="C22" s="22"/>
       <c r="D22" s="6" t="s">
-        <v>359</v>
+        <v>335</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B23" s="22"/>
       <c r="C23" s="22"/>
       <c r="D23" s="6" t="s">
-        <v>360</v>
+        <v>336</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B24" s="22"/>
       <c r="C24" s="22"/>
       <c r="D24" s="6" t="s">
-        <v>361</v>
+        <v>337</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B25" s="22"/>
       <c r="C25" s="22"/>
       <c r="D25" s="6" t="s">
-        <v>362</v>
+        <v>338</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="2:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B26" s="22"/>
       <c r="C26" s="22"/>
       <c r="D26" s="6" t="s">
-        <v>363</v>
+        <v>339</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B27" s="22"/>
       <c r="C27" s="22"/>
       <c r="D27" s="6" t="s">
-        <v>364</v>
+        <v>340</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B28" s="23"/>
       <c r="C28" s="23"/>
       <c r="D28" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E28" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="F28" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="G28" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="G28" s="10" t="s">
+      <c r="H28" s="11" t="s">
         <v>92</v>
-      </c>
-      <c r="H28" s="11" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -3352,7 +3354,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6EAA36F-FB67-40E1-BF91-53944F3B0839}">
   <dimension ref="B2:H19"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3401,22 +3405,22 @@
     </row>
     <row r="4" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B4" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="D4" s="13" t="s">
+      <c r="E4" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="F4" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="G4" s="14" t="s">
         <v>97</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>98</v>
       </c>
       <c r="H4" s="15" t="s">
         <v>13</v>
@@ -3426,16 +3430,16 @@
       <c r="B5" s="22"/>
       <c r="C5" s="22"/>
       <c r="D5" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="G5" s="7" t="s">
         <v>101</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>102</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>13</v>
@@ -3445,16 +3449,16 @@
       <c r="B6" s="22"/>
       <c r="C6" s="22"/>
       <c r="D6" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="G6" s="7" t="s">
         <v>105</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>106</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>13</v>
@@ -3464,16 +3468,16 @@
       <c r="B7" s="22"/>
       <c r="C7" s="22"/>
       <c r="D7" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="F7" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="G7" s="7" t="s">
         <v>109</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>110</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>13</v>
@@ -3483,16 +3487,16 @@
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="G8" s="7" t="s">
         <v>113</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>114</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>13</v>
@@ -3502,16 +3506,16 @@
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
       <c r="D9" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="F9" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="G9" s="7" t="s">
         <v>117</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>118</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>13</v>
@@ -3521,16 +3525,16 @@
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
       <c r="D10" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="F10" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="G10" s="7" t="s">
         <v>121</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>122</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>13</v>
@@ -3540,16 +3544,16 @@
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
       <c r="D11" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="F11" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="G11" s="7" t="s">
         <v>125</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>126</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>13</v>
@@ -3559,16 +3563,16 @@
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="F12" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="G12" s="7" t="s">
         <v>129</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>130</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>13</v>
@@ -3578,16 +3582,16 @@
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="F13" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="G13" s="7" t="s">
         <v>133</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>134</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>13</v>
@@ -3597,16 +3601,16 @@
       <c r="B14" s="22"/>
       <c r="C14" s="22"/>
       <c r="D14" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F14" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="F14" s="7" t="s">
+      <c r="G14" s="7" t="s">
         <v>136</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>137</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>13</v>
@@ -3616,92 +3620,92 @@
       <c r="B15" s="22"/>
       <c r="C15" s="22"/>
       <c r="D15" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="F15" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="G15" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="H15" s="8" t="s">
         <v>141</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="105" x14ac:dyDescent="0.25">
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
       <c r="D16" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="F16" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="G16" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="H16" s="8" t="s">
         <v>146</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
       <c r="D17" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="F17" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="G17" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="H17" s="8" t="s">
         <v>151</v>
-      </c>
-      <c r="H17" s="8" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="285" x14ac:dyDescent="0.25">
       <c r="B18" s="22"/>
       <c r="C18" s="22"/>
       <c r="D18" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="F18" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="G18" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="H18" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="23"/>
       <c r="C19" s="23"/>
       <c r="D19" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="E19" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="F19" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="F19" s="10" t="s">
-        <v>160</v>
-      </c>
       <c r="G19" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H19" s="11" t="s">
         <v>13</v>
@@ -3727,7 +3731,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6A999D4-8369-47DC-9575-F397AA4AC9D4}">
   <dimension ref="B2:H23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3776,269 +3782,269 @@
     </row>
     <row r="4" spans="2:8" ht="300" x14ac:dyDescent="0.25">
       <c r="B4" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="C4" s="22" t="s">
-        <v>161</v>
-      </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="8" t="s">
         <v>165</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="195" x14ac:dyDescent="0.25">
       <c r="B5" s="22"/>
       <c r="C5" s="22"/>
       <c r="D5" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="G5" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="H5" s="8" t="s">
         <v>170</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B6" s="22"/>
       <c r="C6" s="22"/>
       <c r="D6" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="G6" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="H6" s="8" t="s">
         <v>175</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B7" s="22"/>
       <c r="C7" s="22"/>
       <c r="D7" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="F7" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="G7" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="H7" s="8" t="s">
         <v>180</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="G8" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="G8" s="7" t="s">
-        <v>185</v>
-      </c>
       <c r="H8" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
       <c r="D9" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="F9" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="G9" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="G9" s="7" t="s">
-        <v>189</v>
-      </c>
       <c r="H9" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="360" x14ac:dyDescent="0.25">
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
       <c r="D10" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="F10" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="G10" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="G10" s="7" t="s">
-        <v>193</v>
-      </c>
       <c r="H10" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="195" x14ac:dyDescent="0.25">
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
       <c r="D11" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="F11" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="G11" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>197</v>
-      </c>
       <c r="H11" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="150" x14ac:dyDescent="0.25">
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="F12" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="G12" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="H12" s="8" t="s">
         <v>201</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="90" x14ac:dyDescent="0.25">
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="F13" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="G13" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="H13" s="8" t="s">
         <v>206</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="255" x14ac:dyDescent="0.25">
       <c r="B14" s="22"/>
       <c r="C14" s="22"/>
       <c r="D14" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="F14" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="G14" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="H14" s="8" t="s">
         <v>211</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B15" s="22"/>
       <c r="C15" s="22"/>
       <c r="D15" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="F15" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="G15" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="H15" s="8" t="s">
         <v>216</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
       <c r="D16" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="F16" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="G16" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="H16" s="8" t="s">
         <v>221</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="330" x14ac:dyDescent="0.25">
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
       <c r="D17" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="F17" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="G17" s="7" t="s">
         <v>225</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>226</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>49</v>
@@ -4048,114 +4054,114 @@
       <c r="B18" s="22"/>
       <c r="C18" s="22"/>
       <c r="D18" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="F18" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="G18" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="H18" s="8" t="s">
         <v>230</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="165" x14ac:dyDescent="0.25">
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
       <c r="D19" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="F19" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="G19" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="H19" s="8" t="s">
         <v>235</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="165" x14ac:dyDescent="0.25">
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
       <c r="D20" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="F20" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="G20" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="H20" s="8" t="s">
         <v>240</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="22"/>
       <c r="C21" s="22"/>
       <c r="D21" s="6" t="s">
-        <v>352</v>
+        <v>330</v>
       </c>
       <c r="E21" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="G21" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="F21" s="6" t="s">
-        <v>352</v>
-      </c>
-      <c r="G21" s="7" t="s">
+      <c r="H21" s="8" t="s">
         <v>243</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="22"/>
       <c r="C22" s="22"/>
       <c r="D22" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="E22" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="F22" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="G22" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="F22" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>247</v>
-      </c>
       <c r="H22" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="23"/>
       <c r="C23" s="23"/>
       <c r="D23" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="H23" s="11" t="s">
         <v>249</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>248</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>249</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>249</v>
-      </c>
-      <c r="H23" s="11" t="s">
-        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -4178,7 +4184,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03345100-042D-4FEF-ADD8-004BAB1EB1EC}">
   <dimension ref="B2:H32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H20" sqref="D16:H20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4227,117 +4235,117 @@
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="C4" s="25" t="s">
         <v>251</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="D4" s="21" t="s">
         <v>252</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="E4" s="21" t="s">
         <v>253</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="F4" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>256</v>
-      </c>
       <c r="H4" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="120" x14ac:dyDescent="0.25">
       <c r="B5" s="22"/>
       <c r="C5" s="26"/>
       <c r="D5" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>260</v>
-      </c>
       <c r="H5" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="120" x14ac:dyDescent="0.25">
       <c r="B6" s="22"/>
       <c r="C6" s="26"/>
       <c r="D6" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>264</v>
-      </c>
       <c r="H6" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B7" s="22"/>
       <c r="C7" s="26"/>
       <c r="D7" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>268</v>
-      </c>
       <c r="H7" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="240" x14ac:dyDescent="0.25">
       <c r="B8" s="22"/>
       <c r="C8" s="26"/>
       <c r="D8" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="4" t="s">
         <v>272</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="22"/>
       <c r="C9" s="26"/>
       <c r="D9" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>276</v>
-      </c>
       <c r="G9" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>13</v>
@@ -4347,349 +4355,349 @@
       <c r="B10" s="22"/>
       <c r="C10" s="26"/>
       <c r="D10" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="F10" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>280</v>
-      </c>
       <c r="H10" s="4" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" ht="17.25" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="22"/>
       <c r="C11" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="F11" s="7" t="s">
+        <v>496</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>520</v>
+      </c>
+      <c r="H11" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>284</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>285</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="6" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>289</v>
+        <v>491</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>290</v>
+        <v>519</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" ht="17.25" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="6" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>293</v>
+        <v>490</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>294</v>
+        <v>518</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" ht="17.25" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" s="22"/>
       <c r="C14" s="22"/>
       <c r="D14" s="6" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>297</v>
+        <v>497</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>353</v>
+        <v>517</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="75" x14ac:dyDescent="0.25">
       <c r="B15" s="22"/>
       <c r="C15" s="22"/>
       <c r="D15" s="6" t="s">
-        <v>298</v>
+        <v>515</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>298</v>
+        <v>484</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>354</v>
+        <v>516</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
       <c r="D16" s="6" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>302</v>
+        <v>495</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>303</v>
+        <v>514</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="32.25" x14ac:dyDescent="0.25">
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
       <c r="D17" s="6" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>307</v>
+        <v>494</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>308</v>
+        <v>513</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="32.25" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B18" s="22"/>
       <c r="C18" s="22"/>
       <c r="D18" s="6" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>311</v>
+        <v>492</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>312</v>
+        <v>512</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" ht="32.25" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
       <c r="D19" s="6" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>314</v>
+        <v>299</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>315</v>
+        <v>493</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>316</v>
+        <v>511</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="17.25" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="75" x14ac:dyDescent="0.25">
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
       <c r="D20" s="6" t="s">
-        <v>317</v>
+        <v>300</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>318</v>
+        <v>301</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>319</v>
+        <v>489</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>320</v>
+        <v>510</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" ht="17.25" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="75" x14ac:dyDescent="0.25">
       <c r="B21" s="22"/>
       <c r="C21" s="22"/>
       <c r="D21" s="6" t="s">
-        <v>321</v>
+        <v>302</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>322</v>
+        <v>303</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>323</v>
+        <v>500</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>324</v>
+        <v>509</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="22"/>
       <c r="C22" s="22"/>
       <c r="D22" s="6" t="s">
-        <v>326</v>
+        <v>305</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>327</v>
+        <v>306</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>328</v>
+        <v>307</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>329</v>
+        <v>508</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>330</v>
+        <v>308</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="22"/>
       <c r="C23" s="22"/>
       <c r="D23" s="6" t="s">
-        <v>331</v>
+        <v>309</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>332</v>
+        <v>310</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>331</v>
+        <v>309</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>333</v>
+        <v>311</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>330</v>
+        <v>308</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="22"/>
       <c r="C24" s="22"/>
       <c r="D24" s="6" t="s">
-        <v>334</v>
+        <v>312</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>335</v>
+        <v>313</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>334</v>
+        <v>312</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>336</v>
+        <v>314</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>330</v>
+        <v>308</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="22"/>
       <c r="C25" s="22"/>
       <c r="D25" s="6" t="s">
-        <v>337</v>
+        <v>315</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>337</v>
+        <v>315</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>339</v>
+        <v>317</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>330</v>
+        <v>308</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="22"/>
       <c r="C26" s="22"/>
       <c r="D26" s="6" t="s">
-        <v>340</v>
+        <v>318</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>341</v>
+        <v>319</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>340</v>
+        <v>318</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>342</v>
+        <v>320</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>330</v>
+        <v>308</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="23"/>
       <c r="C27" s="23"/>
       <c r="D27" s="9" t="s">
-        <v>343</v>
+        <v>321</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>344</v>
+        <v>322</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>343</v>
+        <v>321</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>345</v>
+        <v>323</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>330</v>
+        <v>308</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B28" s="27" t="s">
-        <v>346</v>
+        <v>324</v>
       </c>
       <c r="C28" s="27"/>
       <c r="D28" s="27"/>
@@ -4700,7 +4708,7 @@
     </row>
     <row r="29" spans="2:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B29" s="28" t="s">
-        <v>347</v>
+        <v>325</v>
       </c>
       <c r="C29" s="28"/>
       <c r="D29" s="28"/>
@@ -4711,7 +4719,7 @@
     </row>
     <row r="30" spans="2:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B30" s="29" t="s">
-        <v>348</v>
+        <v>326</v>
       </c>
       <c r="C30" s="29"/>
       <c r="D30" s="29"/>
@@ -4722,7 +4730,7 @@
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="30" t="s">
-        <v>349</v>
+        <v>327</v>
       </c>
       <c r="C31" s="30"/>
       <c r="D31" s="30"/>
@@ -4733,7 +4741,7 @@
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="30" t="s">
-        <v>356</v>
+        <v>332</v>
       </c>
       <c r="C32" s="30"/>
       <c r="D32" s="30"/>
@@ -4744,6 +4752,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B32:H32"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="B4:B27"/>
     <mergeCell ref="C4:C10"/>
@@ -4754,11 +4767,6 @@
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="B30:H30"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="B32:H32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4768,7 +4776,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFF538FB-4517-403F-8115-DDCB136C443E}">
   <dimension ref="B2:H46"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4817,22 +4827,22 @@
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="31" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>368</v>
+        <v>476</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>367</v>
+        <v>343</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>369</v>
+        <v>344</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>488</v>
+        <v>447</v>
       </c>
       <c r="H4" s="15" t="s">
         <v>13</v>
@@ -4842,16 +4852,16 @@
       <c r="B5" s="32"/>
       <c r="C5" s="32"/>
       <c r="D5" s="7" t="s">
-        <v>371</v>
+        <v>477</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>370</v>
+        <v>345</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>372</v>
+        <v>346</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>488</v>
+        <v>447</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>13</v>
@@ -4861,583 +4871,586 @@
       <c r="B6" s="32"/>
       <c r="C6" s="32"/>
       <c r="D6" s="7" t="s">
-        <v>374</v>
+        <v>478</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>373</v>
+        <v>347</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>375</v>
+        <v>348</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>488</v>
+        <v>447</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B7" s="32"/>
       <c r="C7" s="32"/>
       <c r="D7" s="7" t="s">
-        <v>377</v>
+        <v>479</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>376</v>
+        <v>349</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>378</v>
+        <v>444</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>482</v>
+        <v>136</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="32"/>
       <c r="C8" s="32"/>
       <c r="D8" s="7" t="s">
-        <v>380</v>
+        <v>351</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>379</v>
+        <v>350</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>381</v>
+        <v>352</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>489</v>
+        <v>506</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="32"/>
       <c r="C9" s="32"/>
       <c r="D9" s="7" t="s">
-        <v>383</v>
+        <v>354</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>382</v>
+        <v>353</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>384</v>
+        <v>355</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>490</v>
+        <v>507</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="75" x14ac:dyDescent="0.25">
       <c r="B10" s="32"/>
       <c r="C10" s="32"/>
       <c r="D10" s="7" t="s">
-        <v>386</v>
+        <v>480</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>385</v>
+        <v>356</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>387</v>
+        <v>357</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>483</v>
+        <v>445</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="32"/>
       <c r="C11" s="32"/>
       <c r="D11" s="7" t="s">
-        <v>389</v>
+        <v>481</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>388</v>
+        <v>358</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>390</v>
+        <v>359</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>484</v>
+        <v>446</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>475</v>
+        <v>437</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="75" x14ac:dyDescent="0.25">
       <c r="B12" s="32"/>
       <c r="C12" s="32"/>
       <c r="D12" s="7" t="s">
-        <v>392</v>
+        <v>361</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>391</v>
+        <v>360</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>491</v>
+        <v>448</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>492</v>
+        <v>449</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="32"/>
       <c r="C13" s="32"/>
       <c r="D13" s="7" t="s">
-        <v>394</v>
+        <v>363</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>393</v>
+        <v>362</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>394</v>
+        <v>363</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>394</v>
+        <v>363</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>476</v>
+        <v>438</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="32"/>
       <c r="C14" s="32"/>
       <c r="D14" s="7" t="s">
-        <v>396</v>
+        <v>365</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>395</v>
+        <v>364</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>396</v>
+        <v>365</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>396</v>
+        <v>365</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>476</v>
+        <v>438</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
       <c r="D15" s="7" t="s">
-        <v>398</v>
+        <v>367</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>397</v>
+        <v>366</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>398</v>
+        <v>367</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>398</v>
+        <v>367</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>476</v>
+        <v>438</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="32"/>
       <c r="C16" s="32"/>
       <c r="D16" s="7" t="s">
-        <v>400</v>
+        <v>369</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>399</v>
+        <v>368</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>400</v>
+        <v>369</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>400</v>
+        <v>369</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>476</v>
+        <v>438</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="32"/>
       <c r="C17" s="32"/>
       <c r="D17" s="7" t="s">
-        <v>402</v>
+        <v>371</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>401</v>
+        <v>370</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>402</v>
+        <v>371</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>402</v>
+        <v>371</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>476</v>
+        <v>438</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="32"/>
       <c r="C18" s="32"/>
       <c r="D18" s="7" t="s">
-        <v>404</v>
+        <v>373</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>403</v>
+        <v>372</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>404</v>
+        <v>373</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>404</v>
+        <v>373</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>476</v>
+        <v>438</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B19" s="32"/>
       <c r="C19" s="32"/>
       <c r="D19" s="7" t="s">
-        <v>406</v>
+        <v>375</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>405</v>
+        <v>374</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>493</v>
+        <v>450</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>494</v>
+        <v>451</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B20" s="32"/>
       <c r="C20" s="32"/>
       <c r="D20" s="7" t="s">
-        <v>408</v>
+        <v>377</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>407</v>
+        <v>376</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>499</v>
+        <v>456</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>500</v>
+        <v>457</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="32"/>
       <c r="C21" s="32"/>
       <c r="D21" s="7" t="s">
-        <v>410</v>
+        <v>379</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>409</v>
+        <v>378</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>411</v>
+        <v>485</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>485</v>
+        <v>136</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="32"/>
       <c r="C22" s="32"/>
       <c r="D22" s="7" t="s">
-        <v>413</v>
+        <v>381</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>412</v>
+        <v>380</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>414</v>
+        <v>382</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>496</v>
+        <v>453</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="32"/>
       <c r="C23" s="32"/>
       <c r="D23" s="7" t="s">
-        <v>416</v>
+        <v>384</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>415</v>
+        <v>383</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>416</v>
+        <v>384</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>497</v>
+        <v>454</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B24" s="32"/>
       <c r="C24" s="32"/>
       <c r="D24" s="7" t="s">
-        <v>495</v>
+        <v>452</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>417</v>
+        <v>385</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>495</v>
+        <v>482</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>498</v>
+        <v>455</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>477</v>
+        <v>439</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="32"/>
       <c r="C25" s="32"/>
       <c r="D25" s="7" t="s">
-        <v>419</v>
+        <v>387</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>418</v>
+        <v>386</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>420</v>
+        <v>388</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>501</v>
+        <v>458</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B26" s="32"/>
       <c r="C26" s="32"/>
       <c r="D26" s="7" t="s">
-        <v>504</v>
+        <v>461</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>421</v>
+        <v>389</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>502</v>
+        <v>459</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>503</v>
+        <v>460</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="32"/>
       <c r="C27" s="32"/>
       <c r="D27" s="7" t="s">
-        <v>423</v>
+        <v>391</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>422</v>
+        <v>390</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>423</v>
+        <v>391</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>496</v>
+        <v>453</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="75" x14ac:dyDescent="0.25">
       <c r="B28" s="32"/>
       <c r="C28" s="32"/>
       <c r="D28" s="7" t="s">
-        <v>425</v>
+        <v>393</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>424</v>
+        <v>392</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>505</v>
+        <v>462</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>506</v>
+        <v>463</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="29" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="32"/>
       <c r="C29" s="32"/>
       <c r="D29" s="7" t="s">
-        <v>427</v>
+        <v>395</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>426</v>
+        <v>394</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>427</v>
+        <v>395</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>507</v>
+        <v>464</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="30" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B30" s="32"/>
       <c r="C30" s="32"/>
       <c r="D30" s="7" t="s">
-        <v>429</v>
+        <v>483</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>428</v>
+        <v>396</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>430</v>
+        <v>397</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>508</v>
+        <v>465</v>
       </c>
       <c r="H30" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="32"/>
       <c r="C31" s="32"/>
       <c r="D31" s="7" t="s">
-        <v>432</v>
+        <v>399</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>431</v>
+        <v>398</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>433</v>
+        <v>400</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>486</v>
+        <v>136</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" ht="105" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B32" s="32"/>
       <c r="C32" s="32"/>
       <c r="D32" s="7" t="s">
-        <v>435</v>
+        <v>402</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>434</v>
+        <v>401</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>436</v>
+        <v>403</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>487</v>
+        <v>136</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="150" x14ac:dyDescent="0.25">
       <c r="B33" s="32"/>
       <c r="C33" s="32"/>
       <c r="D33" s="7" t="s">
-        <v>438</v>
+        <v>405</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>437</v>
+        <v>404</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>439</v>
+        <v>486</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>505</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B34" s="32"/>
       <c r="C34" s="32"/>
       <c r="D34" s="7" t="s">
-        <v>441</v>
+        <v>487</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>440</v>
+        <v>406</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>442</v>
+        <v>407</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>509</v>
+        <v>466</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="32"/>
       <c r="C35" s="32"/>
       <c r="D35" s="7" t="s">
-        <v>444</v>
+        <v>409</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>443</v>
+        <v>408</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>445</v>
+        <v>410</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>520</v>
+        <v>475</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="32"/>
       <c r="C36" s="32"/>
       <c r="D36" s="7" t="s">
+        <v>488</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>411</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="G36" s="7" t="s">
         <v>447</v>
-      </c>
-      <c r="E36" s="16" t="s">
-        <v>446</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>448</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>488</v>
       </c>
       <c r="H36" s="8" t="s">
         <v>13</v>
@@ -5447,190 +5460,190 @@
       <c r="B37" s="32"/>
       <c r="C37" s="32"/>
       <c r="D37" s="7" t="s">
-        <v>450</v>
+        <v>414</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>449</v>
+        <v>413</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>451</v>
+        <v>415</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>519</v>
+        <v>474</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="38" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B38" s="32"/>
       <c r="C38" s="32"/>
       <c r="D38" s="7" t="s">
-        <v>453</v>
+        <v>417</v>
       </c>
       <c r="E38" s="16" t="s">
-        <v>452</v>
+        <v>416</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>481</v>
+        <v>443</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>510</v>
+        <v>467</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B39" s="32"/>
       <c r="C39" s="32"/>
       <c r="D39" s="7" t="s">
-        <v>455</v>
+        <v>419</v>
       </c>
       <c r="E39" s="16" t="s">
-        <v>454</v>
+        <v>418</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>456</v>
+        <v>420</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>511</v>
+        <v>468</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="2:8" ht="90" x14ac:dyDescent="0.25">
       <c r="B40" s="32"/>
       <c r="C40" s="32"/>
       <c r="D40" s="7" t="s">
-        <v>458</v>
+        <v>422</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>457</v>
+        <v>421</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>480</v>
+        <v>442</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>512</v>
+        <v>469</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B41" s="32"/>
       <c r="C41" s="32"/>
       <c r="D41" s="7" t="s">
-        <v>460</v>
+        <v>502</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>459</v>
+        <v>423</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>461</v>
+        <v>424</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>517</v>
+        <v>504</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="42" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B42" s="32"/>
       <c r="C42" s="32"/>
       <c r="D42" s="7" t="s">
-        <v>463</v>
+        <v>426</v>
       </c>
       <c r="E42" s="16" t="s">
-        <v>462</v>
+        <v>425</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>464</v>
+        <v>427</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>513</v>
+        <v>470</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="2:8" ht="75" x14ac:dyDescent="0.25">
       <c r="B43" s="32"/>
       <c r="C43" s="32"/>
       <c r="D43" s="7" t="s">
-        <v>466</v>
+        <v>501</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>465</v>
+        <v>428</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>479</v>
+        <v>441</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>518</v>
+        <v>503</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="44" spans="2:8" ht="75" x14ac:dyDescent="0.25">
       <c r="B44" s="32"/>
       <c r="C44" s="32"/>
       <c r="D44" s="7" t="s">
-        <v>468</v>
+        <v>430</v>
       </c>
       <c r="E44" s="16" t="s">
-        <v>467</v>
+        <v>429</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>478</v>
+        <v>440</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>514</v>
+        <v>471</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B45" s="32"/>
       <c r="C45" s="32"/>
       <c r="D45" s="7" t="s">
-        <v>470</v>
+        <v>432</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>469</v>
+        <v>431</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>471</v>
+        <v>433</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>515</v>
+        <v>472</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B46" s="33"/>
       <c r="C46" s="33"/>
       <c r="D46" s="10" t="s">
+        <v>435</v>
+      </c>
+      <c r="E46" s="20" t="s">
+        <v>434</v>
+      </c>
+      <c r="F46" s="10" t="s">
+        <v>436</v>
+      </c>
+      <c r="G46" s="10" t="s">
         <v>473</v>
       </c>
-      <c r="E46" s="20" t="s">
-        <v>472</v>
-      </c>
-      <c r="F46" s="10" t="s">
-        <v>474</v>
-      </c>
-      <c r="G46" s="10" t="s">
-        <v>516</v>
-      </c>
       <c r="H46" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>